<commit_message>
fixing server ip address
</commit_message>
<xml_diff>
--- a/~/upload/myexcel.xlsx
+++ b/~/upload/myexcel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7" count="3">
   <si>
     <t>Table 1</t>
   </si>
@@ -1287,7 +1287,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:G23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -1295,8 +1295,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="7" customWidth="true" style="1" width="16.3516" collapsed="false"/>
+    <col min="8" max="16384" customWidth="true" style="1" width="16.3516" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -1339,11 +1339,11 @@
       <c r="B4" t="s" s="9">
         <v>4</v>
       </c>
-      <c r="C4" s="10">
-        <v>10</v>
+      <c r="C4" s="10" t="n">
+        <v>10.0</v>
       </c>
-      <c r="D4" s="10">
-        <v>10</v>
+      <c r="D4" s="10" t="n">
+        <v>10.0</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
@@ -1354,11 +1354,11 @@
       <c r="B5" t="s" s="9">
         <v>5</v>
       </c>
-      <c r="C5" s="10">
-        <v>20</v>
+      <c r="C5" s="10" t="n">
+        <v>20.0</v>
       </c>
-      <c r="D5" s="10">
-        <v>1000</v>
+      <c r="D5" s="10" t="n">
+        <v>1000.0</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
@@ -1369,11 +1369,11 @@
       <c r="B6" t="s" s="9">
         <v>6</v>
       </c>
-      <c r="C6" s="10">
-        <v>30</v>
+      <c r="C6" s="10" t="n">
+        <v>31.0</v>
       </c>
-      <c r="D6" s="10">
-        <v>10000</v>
+      <c r="D6" s="10" t="n">
+        <v>10000.0</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>

</xml_diff>